<commit_message>
Commit before meeting email
</commit_message>
<xml_diff>
--- a/docs/source/_static/structure/IFDAT_TEMPLATE.xlsx
+++ b/docs/source/_static/structure/IFDAT_TEMPLATE.xlsx
@@ -85,11 +85,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ACC.RVN_" sheetId="76" state="hidden" r:id="rId76"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ACC.EXPNS" sheetId="77" state="visible" r:id="rId77"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ACC.EXPNS_" sheetId="78" state="hidden" r:id="rId78"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ACC.KEY" sheetId="79" state="visible" r:id="rId79"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ACC.KEY_" sheetId="80" state="hidden" r:id="rId80"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CONTENTS'!$A$1:$C$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CONTENTS'!$A$1:$B$39</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -98,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DDTHH:MM:SS"/>
     <numFmt numFmtId="165" formatCode="#,##.00"/>
   </numFmts>
   <fonts count="9">
@@ -289,10 +287,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
@@ -763,7 +761,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -951,7 +949,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -1229,12 +1227,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -19505,12 +19503,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -19801,7 +19799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19809,499 +19807,292 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="40" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>DATASET</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>DATA_SHEET</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>HAS_DATA</t>
         </is>
       </c>
     </row>
     <row r="2" ht="25" customHeight="1">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="3">
         <f>HYPERLINK("#REF.FND!A1", "REF.FND")</f>
         <v/>
       </c>
-      <c r="C2" s="3" t="inlineStr"/>
+      <c r="B2" s="4" t="inlineStr"/>
     </row>
     <row r="3" ht="25" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" s="5">
         <f>HYPERLINK("#REF.FND_DYNMC!A1", "REF.FND_DYNMC")</f>
         <v/>
       </c>
-      <c r="C3" s="2" t="inlineStr"/>
+      <c r="B3" s="2" t="inlineStr"/>
     </row>
     <row r="4" ht="25" customHeight="1">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="3">
         <f>HYPERLINK("#REF.SELF_DBT!A1", "REF.SELF_DBT")</f>
         <v/>
       </c>
-      <c r="C4" s="3" t="inlineStr"/>
+      <c r="B4" s="4" t="inlineStr"/>
     </row>
     <row r="5" ht="25" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B5" s="5">
+      <c r="A5" s="5">
         <f>HYPERLINK("#REF.SELF_DBT_DYNMC!A1", "REF.SELF_DBT_DYNMC")</f>
         <v/>
       </c>
-      <c r="C5" s="2" t="inlineStr"/>
+      <c r="B5" s="2" t="inlineStr"/>
     </row>
     <row r="6" ht="25" customHeight="1">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B6" s="4">
+      <c r="A6" s="3">
         <f>HYPERLINK("#REF.SELF_DBT_OUTSTNDNG_CHNG!A1", "REF.SELF_DBT_OUTSTNDNG_CHNG")</f>
         <v/>
       </c>
-      <c r="C6" s="3" t="inlineStr"/>
+      <c r="B6" s="4" t="inlineStr"/>
     </row>
     <row r="7" ht="25" customHeight="1">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B7" s="5">
+      <c r="A7" s="5">
         <f>HYPERLINK("#REF.SELF_DBT_CPN!A1", "REF.SELF_DBT_CPN")</f>
         <v/>
       </c>
-      <c r="C7" s="2" t="inlineStr"/>
+      <c r="B7" s="2" t="inlineStr"/>
     </row>
     <row r="8" ht="25" customHeight="1">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B8" s="4">
+      <c r="A8" s="3">
         <f>HYPERLINK("#REF.SELF_SHR!A1", "REF.SELF_SHR")</f>
         <v/>
       </c>
-      <c r="C8" s="3" t="inlineStr"/>
+      <c r="B8" s="4" t="inlineStr"/>
     </row>
     <row r="9" ht="25" customHeight="1">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B9" s="5">
+      <c r="A9" s="5">
         <f>HYPERLINK("#REF.SELF_SHR_DYNMC!A1", "REF.SELF_SHR_DYNMC")</f>
         <v/>
       </c>
-      <c r="C9" s="2" t="inlineStr"/>
+      <c r="B9" s="2" t="inlineStr"/>
     </row>
     <row r="10" ht="25" customHeight="1">
-      <c r="A10" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B10" s="4">
+      <c r="A10" s="3">
         <f>HYPERLINK("#REF.SELF_SHR_DVDND!A1", "REF.SELF_SHR_DVDND")</f>
         <v/>
       </c>
-      <c r="C10" s="3" t="inlineStr"/>
+      <c r="B10" s="4" t="inlineStr"/>
     </row>
     <row r="11" ht="25" customHeight="1">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B11" s="5">
+      <c r="A11" s="5">
         <f>HYPERLINK("#REF.SELF_SHR_SPLT!A1", "REF.SELF_SHR_SPLT")</f>
         <v/>
       </c>
-      <c r="C11" s="2" t="inlineStr"/>
+      <c r="B11" s="2" t="inlineStr"/>
     </row>
     <row r="12" ht="25" customHeight="1">
-      <c r="A12" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B12" s="4">
+      <c r="A12" s="3">
         <f>HYPERLINK("#REF.MNGMNT!A1", "REF.MNGMNT")</f>
         <v/>
       </c>
-      <c r="C12" s="3" t="inlineStr"/>
+      <c r="B12" s="4" t="inlineStr"/>
     </row>
     <row r="13" ht="25" customHeight="1">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B13" s="5">
+      <c r="A13" s="5">
         <f>HYPERLINK("#REF.MNGMNT_DYNMC!A1", "REF.MNGMNT_DYNMC")</f>
         <v/>
       </c>
-      <c r="C13" s="2" t="inlineStr"/>
+      <c r="B13" s="2" t="inlineStr"/>
     </row>
     <row r="14" ht="25" customHeight="1">
-      <c r="A14" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" s="3">
         <f>HYPERLINK("#REF.USR!A1", "REF.USR")</f>
         <v/>
       </c>
-      <c r="C14" s="3" t="inlineStr"/>
+      <c r="B14" s="4" t="inlineStr"/>
     </row>
     <row r="15" ht="25" customHeight="1">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B15" s="5">
+      <c r="A15" s="5">
         <f>HYPERLINK("#REF.USR_T_RA!A1", "REF.USR_T_RA")</f>
         <v/>
       </c>
-      <c r="C15" s="2" t="inlineStr"/>
+      <c r="B15" s="2" t="inlineStr"/>
     </row>
     <row r="16" ht="25" customHeight="1">
-      <c r="A16" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B16" s="4">
+      <c r="A16" s="3">
         <f>HYPERLINK("#REF.CNTRPRTY!A1", "REF.CNTRPRTY")</f>
         <v/>
       </c>
-      <c r="C16" s="3" t="inlineStr"/>
+      <c r="B16" s="4" t="inlineStr"/>
     </row>
     <row r="17" ht="25" customHeight="1">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B17" s="5">
+      <c r="A17" s="5">
         <f>HYPERLINK("#REF.DPST!A1", "REF.DPST")</f>
         <v/>
       </c>
-      <c r="C17" s="2" t="inlineStr"/>
+      <c r="B17" s="2" t="inlineStr"/>
     </row>
     <row r="18" ht="25" customHeight="1">
-      <c r="A18" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B18" s="4">
+      <c r="A18" s="3">
         <f>HYPERLINK("#REF.SFT!A1", "REF.SFT")</f>
         <v/>
       </c>
-      <c r="C18" s="3" t="inlineStr"/>
+      <c r="B18" s="4" t="inlineStr"/>
     </row>
     <row r="19" ht="25" customHeight="1">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B19" s="5">
+      <c r="A19" s="5">
         <f>HYPERLINK("#REF.LN!A1", "REF.LN")</f>
         <v/>
       </c>
-      <c r="C19" s="2" t="inlineStr"/>
+      <c r="B19" s="2" t="inlineStr"/>
     </row>
     <row r="20" ht="25" customHeight="1">
-      <c r="A20" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B20" s="4">
+      <c r="A20" s="3">
         <f>HYPERLINK("#REF.DBT!A1", "REF.DBT")</f>
         <v/>
       </c>
-      <c r="C20" s="3" t="inlineStr"/>
+      <c r="B20" s="4" t="inlineStr"/>
     </row>
     <row r="21" ht="25" customHeight="1">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B21" s="5">
+      <c r="A21" s="5">
         <f>HYPERLINK("#REF.SHR!A1", "REF.SHR")</f>
         <v/>
       </c>
-      <c r="C21" s="2" t="inlineStr"/>
+      <c r="B21" s="2" t="inlineStr"/>
     </row>
     <row r="22" ht="25" customHeight="1">
-      <c r="A22" s="3" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B22" s="4">
+      <c r="A22" s="3">
         <f>HYPERLINK("#REF.EDR!A1", "REF.EDR")</f>
         <v/>
       </c>
-      <c r="C22" s="3" t="inlineStr"/>
+      <c r="B22" s="4" t="inlineStr"/>
     </row>
     <row r="23" ht="25" customHeight="1">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>REF</t>
-        </is>
-      </c>
-      <c r="B23" s="5">
+      <c r="A23" s="5">
         <f>HYPERLINK("#REF.ODR!A1", "REF.ODR")</f>
         <v/>
       </c>
-      <c r="C23" s="2" t="inlineStr"/>
+      <c r="B23" s="2" t="inlineStr"/>
     </row>
     <row r="24" ht="25" customHeight="1">
-      <c r="A24" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B24" s="4">
+      <c r="A24" s="3">
         <f>HYPERLINK("#ACC.DPST!A1", "ACC.DPST")</f>
         <v/>
       </c>
-      <c r="C24" s="3" t="inlineStr"/>
+      <c r="B24" s="4" t="inlineStr"/>
     </row>
     <row r="25" ht="25" customHeight="1">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B25" s="5">
+      <c r="A25" s="5">
         <f>HYPERLINK("#ACC.ASST_SFT!A1", "ACC.ASST_SFT")</f>
         <v/>
       </c>
-      <c r="C25" s="2" t="inlineStr"/>
+      <c r="B25" s="2" t="inlineStr"/>
     </row>
     <row r="26" ht="25" customHeight="1">
-      <c r="A26" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B26" s="4">
+      <c r="A26" s="3">
         <f>HYPERLINK("#ACC.ASST_DBT!A1", "ACC.ASST_DBT")</f>
         <v/>
       </c>
-      <c r="C26" s="3" t="inlineStr"/>
+      <c r="B26" s="4" t="inlineStr"/>
     </row>
     <row r="27" ht="25" customHeight="1">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B27" s="5">
+      <c r="A27" s="5">
         <f>HYPERLINK("#ACC.ASST_LN!A1", "ACC.ASST_LN")</f>
         <v/>
       </c>
-      <c r="C27" s="2" t="inlineStr"/>
+      <c r="B27" s="2" t="inlineStr"/>
     </row>
     <row r="28" ht="25" customHeight="1">
-      <c r="A28" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B28" s="4">
+      <c r="A28" s="3">
         <f>HYPERLINK("#ACC.SHR!A1", "ACC.SHR")</f>
         <v/>
       </c>
-      <c r="C28" s="3" t="inlineStr"/>
+      <c r="B28" s="4" t="inlineStr"/>
     </row>
     <row r="29" ht="25" customHeight="1">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B29" s="5">
+      <c r="A29" s="5">
         <f>HYPERLINK("#ACC.EDR!A1", "ACC.EDR")</f>
         <v/>
       </c>
-      <c r="C29" s="2" t="inlineStr"/>
+      <c r="B29" s="2" t="inlineStr"/>
     </row>
     <row r="30" ht="25" customHeight="1">
-      <c r="A30" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B30" s="4">
+      <c r="A30" s="3">
         <f>HYPERLINK("#ACC.ODR!A1", "ACC.ODR")</f>
         <v/>
       </c>
-      <c r="C30" s="3" t="inlineStr"/>
+      <c r="B30" s="4" t="inlineStr"/>
     </row>
     <row r="31" ht="25" customHeight="1">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B31" s="5">
+      <c r="A31" s="5">
         <f>HYPERLINK("#ACC.ASST_NN_FNNCL!A1", "ACC.ASST_NN_FNNCL")</f>
         <v/>
       </c>
-      <c r="C31" s="2" t="inlineStr"/>
+      <c r="B31" s="2" t="inlineStr"/>
     </row>
     <row r="32" ht="25" customHeight="1">
-      <c r="A32" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B32" s="4">
+      <c r="A32" s="3">
         <f>HYPERLINK("#ACC.ASST_RMNNG!A1", "ACC.ASST_RMNNG")</f>
         <v/>
       </c>
-      <c r="C32" s="3" t="inlineStr"/>
+      <c r="B32" s="4" t="inlineStr"/>
     </row>
     <row r="33" ht="25" customHeight="1">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B33" s="5">
+      <c r="A33" s="5">
         <f>HYPERLINK("#ACC.LBLTY_SFT!A1", "ACC.LBLTY_SFT")</f>
         <v/>
       </c>
-      <c r="C33" s="2" t="inlineStr"/>
+      <c r="B33" s="2" t="inlineStr"/>
     </row>
     <row r="34" ht="25" customHeight="1">
-      <c r="A34" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B34" s="4">
+      <c r="A34" s="3">
         <f>HYPERLINK("#ACC.LBLTY_DBT!A1", "ACC.LBLTY_DBT")</f>
         <v/>
       </c>
-      <c r="C34" s="3" t="inlineStr"/>
+      <c r="B34" s="4" t="inlineStr"/>
     </row>
     <row r="35" ht="25" customHeight="1">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B35" s="5">
+      <c r="A35" s="5">
         <f>HYPERLINK("#ACC.LBLTY_LN!A1", "ACC.LBLTY_LN")</f>
         <v/>
       </c>
-      <c r="C35" s="2" t="inlineStr"/>
+      <c r="B35" s="2" t="inlineStr"/>
     </row>
     <row r="36" ht="25" customHeight="1">
-      <c r="A36" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B36" s="4">
+      <c r="A36" s="3">
         <f>HYPERLINK("#ACC.LBLTY_RMNNG!A1", "ACC.LBLTY_RMNNG")</f>
         <v/>
       </c>
-      <c r="C36" s="3" t="inlineStr"/>
+      <c r="B36" s="4" t="inlineStr"/>
     </row>
     <row r="37" ht="25" customHeight="1">
-      <c r="A37" s="2" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B37" s="5">
+      <c r="A37" s="5">
         <f>HYPERLINK("#ACC.HLDR!A1", "ACC.HLDR")</f>
         <v/>
       </c>
-      <c r="C37" s="2" t="inlineStr"/>
+      <c r="B37" s="2" t="inlineStr"/>
     </row>
     <row r="38" ht="25" customHeight="1">
-      <c r="A38" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B38" s="4">
+      <c r="A38" s="3">
         <f>HYPERLINK("#ACC.RVN!A1", "ACC.RVN")</f>
         <v/>
       </c>
-      <c r="C38" s="3" t="inlineStr"/>
+      <c r="B38" s="4" t="inlineStr"/>
     </row>
     <row r="39" ht="25" customHeight="1">
-      <c r="A39" s="2" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B39" s="5">
+      <c r="A39" s="5">
         <f>HYPERLINK("#ACC.EXPNS!A1", "ACC.EXPNS")</f>
         <v/>
       </c>
-      <c r="C39" s="2" t="inlineStr"/>
-    </row>
-    <row r="40" ht="25" customHeight="1">
-      <c r="A40" s="3" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="B40" s="4">
-        <f>HYPERLINK("#ACC.KEY!A1", "ACC.KEY")</f>
-        <v/>
-      </c>
-      <c r="C40" s="3" t="inlineStr"/>
+      <c r="B39" s="2" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C40"/>
+  <autoFilter ref="A1:B39"/>
   <dataValidations count="1">
-    <dataValidation sqref="C2:C40" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B39" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"True"</formula1>
     </dataValidation>
   </dataValidations>
@@ -20326,17 +20117,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -21194,7 +20985,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -22319,12 +22110,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -22529,12 +22320,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -23511,17 +23302,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -24001,12 +23792,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -24476,12 +24267,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -24999,12 +24790,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -25440,7 +25231,7 @@
       <formula1>'REF.SHR_'!$A$1:$A$42</formula1>
     </dataValidation>
     <dataValidation sqref="E4:E5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'REF.SHR_'!$B$1:$B$5</formula1>
+      <formula1>'REF.SHR_'!$B$1:$B$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25464,12 +25255,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>F511</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -25481,7 +25272,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>F512</t>
+          <t>F511</t>
         </is>
       </c>
     </row>
@@ -25493,7 +25284,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>F519</t>
+          <t>F512</t>
         </is>
       </c>
     </row>
@@ -25505,7 +25296,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>F521</t>
+          <t>F519</t>
         </is>
       </c>
     </row>
@@ -25517,7 +25308,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>F522</t>
+          <t>F521</t>
         </is>
       </c>
     </row>
@@ -25525,6 +25316,11 @@
       <c r="A6" t="inlineStr">
         <is>
           <t>CAD</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>F522</t>
         </is>
       </c>
     </row>
@@ -25962,17 +25758,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -44271,12 +44067,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -44745,7 +44541,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -45539,7 +45335,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -45949,7 +45745,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -46342,7 +46138,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -46755,7 +46551,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -47145,7 +46941,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -47515,62 +47311,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -47871,7 +47667,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -48277,17 +48073,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -49353,12 +49149,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -49753,7 +49549,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -50153,7 +49949,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -50535,7 +50331,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -50575,10 +50371,9 @@
     <col width="13.5" customWidth="1" min="27" max="27"/>
     <col width="20.25" customWidth="1" min="28" max="28"/>
     <col width="13.5" customWidth="1" min="29" max="29"/>
-    <col width="13.5" customWidth="1" min="30" max="30"/>
-    <col width="16.2" customWidth="1" min="31" max="31"/>
-    <col width="18.9" customWidth="1" min="32" max="32"/>
-    <col width="13.5" customWidth="1" min="33" max="33"/>
+    <col width="16.2" customWidth="1" min="30" max="30"/>
+    <col width="18.9" customWidth="1" min="31" max="31"/>
+    <col width="13.5" customWidth="1" min="32" max="32"/>
   </cols>
   <sheetData>
     <row r="1" ht="60" customHeight="1">
@@ -50616,8 +50411,7 @@
       <c r="AC1" s="8" t="n"/>
       <c r="AD1" s="8" t="n"/>
       <c r="AE1" s="8" t="n"/>
-      <c r="AF1" s="8" t="n"/>
-      <c r="AG1" s="9" t="n"/>
+      <c r="AF1" s="9" t="n"/>
     </row>
     <row r="2" ht="60" customHeight="1">
       <c r="A2" s="10" t="inlineStr">
@@ -50659,8 +50453,7 @@
       <c r="AC2" s="8" t="n"/>
       <c r="AD2" s="8" t="n"/>
       <c r="AE2" s="8" t="n"/>
-      <c r="AF2" s="8" t="n"/>
-      <c r="AG2" s="9" t="n"/>
+      <c r="AF2" s="9" t="n"/>
     </row>
     <row r="3" ht="60" customHeight="1">
       <c r="A3" s="10" t="inlineStr">
@@ -50810,20 +50603,15 @@
       </c>
       <c r="AD3" s="7" t="inlineStr">
         <is>
-          <t>CFI</t>
+          <t>RSTRCTRD_T</t>
         </is>
       </c>
       <c r="AE3" s="7" t="inlineStr">
         <is>
-          <t>RSTRCTRD_T</t>
+          <t>RSTRCTRD_FRM</t>
         </is>
       </c>
       <c r="AF3" s="7" t="inlineStr">
-        <is>
-          <t>RSTRCTRD_FRM</t>
-        </is>
-      </c>
-      <c r="AG3" s="7" t="inlineStr">
         <is>
           <t>ALS_OF</t>
         </is>
@@ -50862,7 +50650,6 @@
       <c r="AD4" s="14" t="n"/>
       <c r="AE4" s="14" t="n"/>
       <c r="AF4" s="14" t="n"/>
-      <c r="AG4" s="14" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="12" t="n"/>
@@ -50897,12 +50684,11 @@
       <c r="AD5" s="14" t="n"/>
       <c r="AE5" s="14" t="n"/>
       <c r="AF5" s="14" t="n"/>
-      <c r="AG5" s="14" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:AG1"/>
-    <mergeCell ref="B2:AG2"/>
+    <mergeCell ref="B1:AF1"/>
+    <mergeCell ref="B2:AF2"/>
   </mergeCells>
   <dataValidations count="14">
     <dataValidation sqref="E4:E5 S4:S5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
@@ -50969,7 +50755,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -51352,12 +51138,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -51797,7 +51583,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -52168,12 +51954,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -52569,12 +52355,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -52867,112 +52653,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="16.2" customWidth="1" min="1" max="1"/>
-    <col width="16.2" customWidth="1" min="2" max="2"/>
-    <col width="16.2" customWidth="1" min="3" max="3"/>
-    <col width="13.5" customWidth="1" min="4" max="4"/>
-    <col width="13.5" customWidth="1" min="5" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="60" customHeight="1">
-      <c r="A1" s="6">
-        <f>HYPERLINK("#CONTENTS!A1", "CONTENTS")</f>
-        <v/>
-      </c>
-      <c r="B1" s="8" t="n"/>
-      <c r="C1" s="9" t="n"/>
-      <c r="D1" s="7" t="inlineStr"/>
-      <c r="E1" s="9" t="n"/>
-    </row>
-    <row r="2" ht="60" customHeight="1">
-      <c r="A2" s="10" t="inlineStr">
-        <is>
-          <t>DIMENSIONS</t>
-        </is>
-      </c>
-      <c r="B2" s="8" t="n"/>
-      <c r="C2" s="9" t="n"/>
-      <c r="D2" s="11" t="inlineStr">
-        <is>
-          <t>MEASURES</t>
-        </is>
-      </c>
-      <c r="E2" s="9" t="n"/>
-    </row>
-    <row r="3" ht="60" customHeight="1">
-      <c r="A3" s="10" t="inlineStr">
-        <is>
-          <t>IID</t>
-        </is>
-      </c>
-      <c r="B3" s="10" t="inlineStr">
-        <is>
-          <t>DT</t>
-        </is>
-      </c>
-      <c r="C3" s="10" t="inlineStr">
-        <is>
-          <t>FRQNCY</t>
-        </is>
-      </c>
-      <c r="D3" s="7" t="inlineStr">
-        <is>
-          <t>BK_PRC</t>
-        </is>
-      </c>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t>INCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="12" t="n"/>
-      <c r="B4" s="15" t="n"/>
-      <c r="C4" s="12" t="n"/>
-      <c r="D4" s="16" t="n"/>
-      <c r="E4" s="16" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="12" t="n"/>
-      <c r="B5" s="15" t="n"/>
-      <c r="C5" s="12" t="n"/>
-      <c r="D5" s="16" t="n"/>
-      <c r="E5" s="16" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation sqref="C4:C5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.KEY_'!$A$1:$A$35</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -52994,57 +52674,57 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>.</t>
         </is>
       </c>
     </row>
@@ -71381,270 +71061,6 @@
       <c r="B2554" t="inlineStr">
         <is>
           <t>ZODM</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Q</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>A3</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>A4</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>A10</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>A20</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>A30</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>A_3</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>M2</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>M_2</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>M_3</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>W2</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>W3</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>W4</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>W_2</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>W_3</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>D_2</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>H3</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>OA</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>OM</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>_O</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>_U</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>_Z</t>
         </is>
       </c>
     </row>

</xml_diff>